<commit_message>
data results for sonar
</commit_message>
<xml_diff>
--- a/3_2.2_Sonar/Sonar_results.xlsx
+++ b/3_2.2_Sonar/Sonar_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t xml:space="preserve">Min reliable depth</t>
   </si>
@@ -49,7 +49,37 @@
     <t xml:space="preserve">Theoretical</t>
   </si>
   <si>
+    <t xml:space="preserve">Point of overflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">actual distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perpendicular length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US reading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">angle deviation</t>
+  </si>
+  <si>
     <t xml:space="preserve">inf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measurement at 40cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean dev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">st. dev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measurement at 100cm</t>
   </si>
 </sst>
 </file>
@@ -62,11 +92,12 @@
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -82,6 +113,17 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,7 +168,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -136,6 +178,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -245,6 +291,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -554,17 +601,17 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="91098540"/>
-        <c:axId val="35031387"/>
+        <c:axId val="59845567"/>
+        <c:axId val="59697877"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91098540"/>
+        <c:axId val="59845567"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -593,12 +640,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35031387"/>
+        <c:crossAx val="59697877"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="35031387"/>
+        <c:axId val="59697877"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -613,7 +660,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -642,7 +689,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91098540"/>
+        <c:crossAx val="59845567"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -684,15 +731,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>250560</xdr:colOff>
+      <xdr:colOff>250920</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>598320</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>597960</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:rowOff>35640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -700,8 +747,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6900840" y="325800"/>
-        <a:ext cx="5224320" cy="3936600"/>
+        <a:off x="6794280" y="325800"/>
+        <a:ext cx="7019280" cy="3936240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -719,16 +766,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:J78"/>
+  <dimension ref="A2:P78"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M74" activeCellId="0" sqref="M74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="12" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.9030612244898"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.3928571428571"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="14.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1365,6 +1416,9 @@
         <f aca="false">50/(COS(I42*PI()/180))</f>
         <v>65.2703644666139</v>
       </c>
+      <c r="M42" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
@@ -1391,6 +1445,18 @@
         <f aca="false">50/(COS(I43*PI()/180))</f>
         <v>70.7106781186547</v>
       </c>
+      <c r="M43" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="N43" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="O43" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="P43" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
@@ -1414,6 +1480,19 @@
         <f aca="false">50/(COS(I44*PI()/180))</f>
         <v>77.7861913430206</v>
       </c>
+      <c r="M44" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="N44" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="O44" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="P44" s="3" t="n">
+        <f aca="false">DEGREES(ACOS(N44/M44))</f>
+        <v>31.5198585798836</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
@@ -1437,6 +1516,19 @@
         <f aca="false">50/(COS(I45*PI()/180))</f>
         <v>100</v>
       </c>
+      <c r="M45" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="N45" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="O45" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="P45" s="3" t="n">
+        <f aca="false">DEGREES(ACOS(N45/M45))</f>
+        <v>80.1031465571841</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
@@ -1460,6 +1552,19 @@
         <f aca="false">50/(COS(I46*PI()/180))</f>
         <v>146.190220008154</v>
       </c>
+      <c r="M46" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="N46" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="O46" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="P46" s="3" t="n">
+        <f aca="false">DEGREES(ACOS(N46/M46))</f>
+        <v>39.4005687537377</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
@@ -1483,6 +1588,19 @@
         <f aca="false">50/(COS(I47*PI()/180))</f>
         <v>287.938524157182</v>
       </c>
+      <c r="M47" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="N47" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="O47" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="P47" s="3" t="n">
+        <f aca="false">DEGREES(ACOS(N47/M47))</f>
+        <v>39.0933679778365</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
@@ -1502,8 +1620,21 @@
       <c r="I48" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="J48" s="3" t="s">
-        <v>9</v>
+      <c r="J48" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M48" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="N48" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="O48" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="P48" s="3" t="n">
+        <f aca="false">DEGREES(ACOS(N48/M48))</f>
+        <v>42.6679254941084</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1625,6 +1756,9 @@
       <c r="B58" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="E58" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
@@ -1633,6 +1767,13 @@
       <c r="B59" s="0" t="n">
         <v>40</v>
       </c>
+      <c r="E59" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F59" s="0" t="n">
+        <f aca="false">AVERAGE(B59:B68)</f>
+        <v>40.5</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
@@ -1641,6 +1782,13 @@
       <c r="B60" s="0" t="n">
         <v>40</v>
       </c>
+      <c r="E60" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F60" s="0" t="n">
+        <f aca="false">F59-40</f>
+        <v>0.5</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
@@ -1649,6 +1797,13 @@
       <c r="B61" s="0" t="n">
         <v>40</v>
       </c>
+      <c r="E61" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F61" s="0" t="n">
+        <f aca="false">STDEV(B59:B68)</f>
+        <v>0.52704627669473</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
@@ -1665,6 +1820,9 @@
       <c r="B63" s="0" t="n">
         <v>41</v>
       </c>
+      <c r="E63" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
@@ -1673,6 +1831,13 @@
       <c r="B64" s="0" t="n">
         <v>40</v>
       </c>
+      <c r="E64" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F64" s="0" t="n">
+        <f aca="false">AVERAGE(B69:B78)</f>
+        <v>101.5</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
@@ -1681,6 +1846,13 @@
       <c r="B65" s="0" t="n">
         <v>40</v>
       </c>
+      <c r="E65" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F65" s="0" t="n">
+        <f aca="false">F64-100</f>
+        <v>1.5</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
@@ -1688,6 +1860,13 @@
       </c>
       <c r="B66" s="0" t="n">
         <v>41</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F66" s="0" t="n">
+        <f aca="false">STDEV(B69:B78)</f>
+        <v>0.52704627669473</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>